<commit_message>
Subo ej5 y 2
</commit_message>
<xml_diff>
--- a/practica 2/diagramas/Ejer 3 diagramas.xlsx
+++ b/practica 2/diagramas/Ejer 3 diagramas.xlsx
@@ -1,27 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin\Desktop\facu\2do\2do semestre\iso\practica 2\diagramas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguspc\Desktop\facu\2do\2do semestre\ISO\practica 2\diagramas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA35AEB-F9C9-44CD-9C1B-4BB95093D70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D375055D-C0CE-45DF-9B75-73D211AC960B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA347444-6128-45C2-8F04-F69AB096F0DE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA347444-6128-45C2-8F04-F69AB096F0DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -252,9 +260,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -292,7 +300,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -398,7 +406,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -540,7 +548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -550,23 +558,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC85E06-74CE-4471-A58D-3575DC7372BC}">
   <dimension ref="A1:BA26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AY28" sqref="AY28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="50" width="3.5703125" customWidth="1"/>
-    <col min="51" max="53" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="5" max="50" width="3.5546875" customWidth="1"/>
+    <col min="51" max="51" width="3.6640625" customWidth="1"/>
+    <col min="52" max="52" width="4.77734375" customWidth="1"/>
+    <col min="53" max="53" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -727,7 +737,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -806,7 +816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -903,7 +913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -994,7 +1004,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1069,7 +1079,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1154,7 +1164,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
@@ -1209,20 +1219,19 @@
       <c r="AX8" s="5"/>
       <c r="AY8" s="5"/>
       <c r="AZ8" s="8">
-        <f>ROUND(AVERAGE(AZ3,AZ7),1)</f>
-        <v>27</v>
+        <v>29.6</v>
       </c>
       <c r="BA8" s="8">
         <f>ROUND(AVERAGE(BA3,BA7),1)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +1392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -1464,7 +1473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1561,7 +1570,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1652,7 +1661,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1725,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1810,7 +1819,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>23</v>
       </c>
@@ -1865,20 +1874,18 @@
       <c r="AX17" s="5"/>
       <c r="AY17" s="5"/>
       <c r="AZ17" s="8">
-        <f>ROUND(AVERAGE(AZ12,AZ16),1)</f>
-        <v>15.5</v>
+        <v>22.8</v>
       </c>
       <c r="BA17" s="8">
-        <f>ROUND(AVERAGE(BA12,BA16),1)</f>
-        <v>7.5</v>
+        <v>13.4</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2039,7 +2046,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -2118,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
@@ -2215,7 +2222,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
@@ -2306,7 +2313,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -2381,7 +2388,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -2466,7 +2473,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>26</v>
       </c>
@@ -2549,12 +2556,10 @@
       <c r="AX26" s="5"/>
       <c r="AY26" s="5"/>
       <c r="AZ26" s="8">
-        <f>ROUND(AVERAGE(AZ21,AZ25),1)</f>
-        <v>24</v>
+        <v>30.8</v>
       </c>
       <c r="BA26" s="8">
-        <f>ROUND(AVERAGE(BA21,BA25),1)</f>
-        <v>17.5</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>